<commit_message>
Yazım.Düzeni  Büyük Harf Küçük Harf Tekrar Eden Verileri BUL SİL KALDIR
</commit_message>
<xml_diff>
--- a/working 13.xlsx
+++ b/working 13.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EXCELDEKİ GENEL HATALAR" sheetId="1" r:id="rId1"/>
@@ -182,8 +182,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="169" formatCode="_-[$₺-41F]* #,##0.00_-;\-[$₺-41F]* #,##0.00_-;_-[$₺-41F]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="_-[$₺-41F]* #,##0.00_-;\-[$₺-41F]* #,##0.00_-;_-[$₺-41F]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -410,21 +410,9 @@
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -433,13 +421,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -452,9 +455,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,163 +756,163 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="7" t="e">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="3" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="4" t="e">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="2" t="e">
         <v>#NAME?</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="7" t="e">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="3" t="e">
         <v>#REF!</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="4" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="7" t="e">
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="3" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="4" t="e">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="2" t="e">
         <v>#NULL!</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="7" t="e">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="3" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -966,7 +966,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="str">
@@ -988,13 +988,13 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="5">
         <v>45040</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="6">
         <v>0.4368055555555555</v>
       </c>
       <c r="K15" t="s">
@@ -1069,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1084,186 +1084,186 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>2018</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>300</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>2018</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>400</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>2018</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>100</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>2018</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>200</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>2018</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>320</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>2018</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>350</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="12">
         <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>2018</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>222</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1">
         <v>2018</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>400</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="12">
         <v>90</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
         <v>2018</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>200</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="12">
         <v>80</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19" t="str">
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22" t="str">
         <f>IF(AVERAGE(F3:F11)&gt;=105,"Satış Başarılı","Satış Başarısız")</f>
         <v>Satış Başarısız</v>
       </c>
-      <c r="F12" s="20"/>
+      <c r="F12" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1279,269 +1279,269 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="3"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="13">
         <v>12.5</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="13">
         <v>8</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="13">
         <v>20.5</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="13">
         <v>10.5</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="13">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="13">
         <v>7.6</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="13">
         <v>6.2999999999999989</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="13">
         <v>12.5</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="13">
         <v>12.8</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="13">
         <v>2.6999999999999997</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="13">
         <v>10.8</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="13">
         <v>7.2000000000000011</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="13">
         <v>1.5</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="13">
         <v>1</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="13">
         <v>18.600000000000001</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="13">
         <v>6.3999999999999986</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="13">
         <v>17.5</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="13">
         <v>12</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="13">
         <v>6.4</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="13">
         <v>26.95</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="13">
         <v>0.79999999999999982</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="13">
         <v>2.1000000000000005</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="13">
         <v>9</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="13">
         <v>6.4</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="13">
         <v>25.2</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="13">
         <f>Sayfa3!B6</f>
         <v>12.5</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="13">
         <f>Sayfa3!C6</f>
         <v>8</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="13">
         <f>Sayfa3!D6</f>
         <v>20.5</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="13">
         <f>Sayfa3!E6</f>
         <v>10.5</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="13">
         <f>Sayfa3!F6</f>
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="13">
         <f>Sayfa3!B7</f>
         <v>10.4</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="13">
         <f>Sayfa3!C7</f>
         <v>6.2999999999999989</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="13">
         <f>Sayfa3!D7</f>
         <v>12.5</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="13">
         <f>Sayfa3!E7</f>
         <v>12.8</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="13">
         <f>Sayfa3!F7</f>
         <v>2.6999999999999997</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="13">
         <f>Sayfa3!B8</f>
         <v>10.8</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="13">
         <f>Sayfa3!C8</f>
         <v>7.2000000000000011</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="13">
         <f>Sayfa3!D8</f>
         <v>1.5</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="13">
         <f>Sayfa3!E8</f>
         <v>1</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="13">
         <f>Sayfa3!F8</f>
         <v>18.600000000000001</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="13">
         <f>Sayfa3!B9</f>
         <v>6.3999999999999986</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="13">
         <f>Sayfa3!C9</f>
         <v>17.5</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="13">
         <f>Sayfa3!D9</f>
         <v>12</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="13">
         <f>Sayfa3!E9</f>
         <v>6.4</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="13">
         <f>Sayfa3!F9</f>
         <v>26.95</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="13">
         <f>Sayfa3!B10</f>
         <v>0.79999999999999982</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="13">
         <f>Sayfa3!C10</f>
         <v>2.1000000000000005</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="13">
         <f>Sayfa3!D10</f>
         <v>9</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="13">
         <f>Sayfa3!E10</f>
         <v>6.4</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="13">
         <f>Sayfa3!F10</f>
         <v>25.2</v>
       </c>
@@ -1626,60 +1626,60 @@
       <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="14">
         <f>P6-(P6*I6)</f>
         <v>12.5</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="14">
         <f t="shared" ref="C6:F6" si="0">Q6-(Q6*J6)</f>
         <v>8</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="14">
         <f t="shared" si="0"/>
         <v>20.5</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="14">
         <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="14">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="13">
         <v>0.5</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="13">
         <v>0.5</v>
       </c>
-      <c r="K6" s="21">
+      <c r="K6" s="13">
         <v>0.5</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="13">
         <v>0.5</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="13">
         <v>0.5</v>
       </c>
       <c r="O6" t="s">
         <v>26</v>
       </c>
-      <c r="P6" s="23">
+      <c r="P6" s="15">
         <v>25</v>
       </c>
-      <c r="Q6" s="23">
+      <c r="Q6" s="15">
         <v>16</v>
       </c>
-      <c r="R6" s="23">
+      <c r="R6" s="15">
         <v>41</v>
       </c>
-      <c r="S6" s="23">
+      <c r="S6" s="15">
         <v>21</v>
       </c>
-      <c r="T6" s="23">
+      <c r="T6" s="15">
         <v>44</v>
       </c>
     </row>
@@ -1687,60 +1687,60 @@
       <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="14">
         <f t="shared" ref="B7:B11" si="1">P7-(P7*I7)</f>
         <v>10.4</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="14">
         <f t="shared" ref="C7:C11" si="2">Q7-(Q7*J7)</f>
         <v>6.2999999999999989</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="14">
         <f t="shared" ref="D7:D11" si="3">R7-(R7*K7)</f>
         <v>12.5</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="14">
         <f t="shared" ref="E7:E11" si="4">S7-(S7*L7)</f>
         <v>12.8</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="14">
         <f t="shared" ref="F7:F11" si="5">T7-(T7*M7)</f>
         <v>2.6999999999999997</v>
       </c>
       <c r="H7" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="13">
         <v>0.6</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="K7" s="21">
+      <c r="K7" s="13">
         <v>0.5</v>
       </c>
-      <c r="L7" s="21">
+      <c r="L7" s="13">
         <v>0.6</v>
       </c>
-      <c r="M7" s="21">
+      <c r="M7" s="13">
         <v>0.55000000000000004</v>
       </c>
       <c r="O7" t="s">
         <v>25</v>
       </c>
-      <c r="P7" s="23">
+      <c r="P7" s="15">
         <v>26</v>
       </c>
-      <c r="Q7" s="23">
+      <c r="Q7" s="15">
         <v>14</v>
       </c>
-      <c r="R7" s="23">
+      <c r="R7" s="15">
         <v>25</v>
       </c>
-      <c r="S7" s="23">
+      <c r="S7" s="15">
         <v>32</v>
       </c>
-      <c r="T7" s="23">
+      <c r="T7" s="15">
         <v>6</v>
       </c>
     </row>
@@ -1748,60 +1748,60 @@
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="14">
         <f t="shared" si="1"/>
         <v>10.8</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="14">
         <f t="shared" si="2"/>
         <v>7.2000000000000011</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="14">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="14">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="14">
         <f t="shared" si="5"/>
         <v>18.600000000000001</v>
       </c>
       <c r="H8" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="13">
         <v>0.7</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="13">
         <v>0.6</v>
       </c>
-      <c r="K8" s="21">
+      <c r="K8" s="13">
         <v>0.5</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="13">
         <v>0.5</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="13">
         <v>0.4</v>
       </c>
       <c r="O8" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="23">
+      <c r="P8" s="15">
         <v>36</v>
       </c>
-      <c r="Q8" s="23">
+      <c r="Q8" s="15">
         <v>18</v>
       </c>
-      <c r="R8" s="23">
+      <c r="R8" s="15">
         <v>3</v>
       </c>
-      <c r="S8" s="23">
+      <c r="S8" s="15">
         <v>2</v>
       </c>
-      <c r="T8" s="23">
+      <c r="T8" s="15">
         <v>31</v>
       </c>
     </row>
@@ -1809,60 +1809,60 @@
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="14">
         <f t="shared" si="1"/>
         <v>6.3999999999999986</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="14">
         <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="14">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="14">
         <f t="shared" si="4"/>
         <v>6.4</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="14">
         <f t="shared" si="5"/>
         <v>26.95</v>
       </c>
       <c r="H9" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="13">
         <v>0.8</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="13">
         <v>0.65</v>
       </c>
-      <c r="K9" s="21">
+      <c r="K9" s="13">
         <v>0.5</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="13">
         <v>0.6</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="13">
         <v>0.45</v>
       </c>
       <c r="O9" t="s">
         <v>28</v>
       </c>
-      <c r="P9" s="23">
+      <c r="P9" s="15">
         <v>32</v>
       </c>
-      <c r="Q9" s="23">
+      <c r="Q9" s="15">
         <v>50</v>
       </c>
-      <c r="R9" s="23">
+      <c r="R9" s="15">
         <v>24</v>
       </c>
-      <c r="S9" s="23">
+      <c r="S9" s="15">
         <v>16</v>
       </c>
-      <c r="T9" s="23">
+      <c r="T9" s="15">
         <v>49</v>
       </c>
     </row>
@@ -1870,60 +1870,60 @@
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="14">
         <f t="shared" si="1"/>
         <v>0.79999999999999982</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="14">
         <f t="shared" si="2"/>
         <v>2.1000000000000005</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="14">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="14">
         <f t="shared" si="4"/>
         <v>6.4</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="14">
         <f t="shared" si="5"/>
         <v>25.2</v>
       </c>
       <c r="H10" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="13">
         <v>0.9</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="13">
         <v>0.7</v>
       </c>
-      <c r="K10" s="21">
+      <c r="K10" s="13">
         <v>0.5</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="13">
         <v>0.6</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="13">
         <v>0.4</v>
       </c>
       <c r="O10" t="s">
         <v>29</v>
       </c>
-      <c r="P10" s="23">
+      <c r="P10" s="15">
         <v>8</v>
       </c>
-      <c r="Q10" s="23">
+      <c r="Q10" s="15">
         <v>7</v>
       </c>
-      <c r="R10" s="23">
+      <c r="R10" s="15">
         <v>18</v>
       </c>
-      <c r="S10" s="23">
+      <c r="S10" s="15">
         <v>16</v>
       </c>
-      <c r="T10" s="23">
+      <c r="T10" s="15">
         <v>42</v>
       </c>
     </row>
@@ -1931,60 +1931,60 @@
       <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="14">
         <f t="shared" si="1"/>
         <v>2.3999999999999986</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="14">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="14">
         <f t="shared" si="3"/>
         <v>6.5</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="14">
         <f t="shared" si="4"/>
         <v>8.36</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="14">
         <f t="shared" si="5"/>
         <v>13.23</v>
       </c>
       <c r="H11" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="13">
         <v>0.9</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="13">
         <v>0.75</v>
       </c>
-      <c r="K11" s="21">
+      <c r="K11" s="13">
         <v>0.5</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="13">
         <v>0.62</v>
       </c>
-      <c r="M11" s="21">
+      <c r="M11" s="13">
         <v>0.37</v>
       </c>
       <c r="O11" t="s">
         <v>36</v>
       </c>
-      <c r="P11" s="23">
+      <c r="P11" s="15">
         <v>24</v>
       </c>
-      <c r="Q11" s="23">
+      <c r="Q11" s="15">
         <v>8</v>
       </c>
-      <c r="R11" s="23">
+      <c r="R11" s="15">
         <v>13</v>
       </c>
-      <c r="S11" s="23">
+      <c r="S11" s="15">
         <v>22</v>
       </c>
-      <c r="T11" s="23">
+      <c r="T11" s="15">
         <v>21</v>
       </c>
     </row>

</xml_diff>